<commit_message>
Added threaded mounting holes to bottom of case.
</commit_message>
<xml_diff>
--- a/acquisition_board_case/acquisition_board_case_BOM.xlsx
+++ b/acquisition_board_case/acquisition_board_case_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Hardware development\pyPhotometry\hardware\acquisition board case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Dropbox\Hardware development\pyPhotometry\hardware\acquisition_board_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D96313D-71AB-4084-9202-62B785A009B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA2005F-D832-41C6-ACBF-8B676E9C867B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +430,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>